<commit_message>
Refactor code for API generation and update Peripheral usage
</commit_message>
<xml_diff>
--- a/NeoPixelClock_Hardware/Documentation/stm32f407vgtx/NPC Peripherals usage.xlsx
+++ b/NeoPixelClock_Hardware/Documentation/stm32f407vgtx/NPC Peripherals usage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Modules</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>PORT</t>
+  </si>
+  <si>
+    <t>Screen</t>
+  </si>
+  <si>
+    <t>PA0,PE0,PC8-12,PD11-15</t>
+  </si>
+  <si>
+    <t>SPI3</t>
   </si>
 </sst>
 </file>
@@ -103,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +158,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF5EF77"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -165,45 +180,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,239 +535,264 @@
   <dimension ref="B3:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="18" width="5.7109375" customWidth="1"/>
+    <col min="3" max="18" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="2">
         <v>2</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="2">
         <v>3</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="2">
         <v>4</v>
       </c>
-      <c r="G13" s="4">
+      <c r="H13" s="2">
         <v>5</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="2">
         <v>6</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J13" s="2">
         <v>7</v>
       </c>
-      <c r="J13" s="4">
+      <c r="K13" s="2">
         <v>8</v>
       </c>
-      <c r="K13" s="4">
+      <c r="L13" s="2">
         <v>9</v>
       </c>
-      <c r="L13" s="4">
+      <c r="M13" s="2">
         <v>10</v>
       </c>
-      <c r="M13" s="4">
+      <c r="N13" s="2">
         <v>11</v>
       </c>
-      <c r="N13" s="4">
+      <c r="O13" s="2">
         <v>12</v>
       </c>
-      <c r="O13" s="4">
+      <c r="P13" s="2">
         <v>13</v>
       </c>
-      <c r="P13" s="4">
+      <c r="Q13" s="2">
         <v>14</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="R13" s="2">
         <v>15</v>
       </c>
     </row>
@@ -756,41 +800,60 @@
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="11"/>
+      <c r="C14" s="17"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C18" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="23">
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="L9:R9"/>
+    <mergeCell ref="B12:R12"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="D6:K6"/>
     <mergeCell ref="D7:K7"/>
     <mergeCell ref="D8:K8"/>
-    <mergeCell ref="B12:Q12"/>
     <mergeCell ref="L3:R3"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="L5:R5"/>
@@ -803,11 +866,6 @@
     <mergeCell ref="D4:K4"/>
     <mergeCell ref="D5:K5"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Hardware Design folder
</commit_message>
<xml_diff>
--- a/NeoPixelClock_Hardware/Documentation/stm32f407vgtx/NPC Peripherals usage.xlsx
+++ b/NeoPixelClock_Hardware/Documentation/stm32f407vgtx/NPC Peripherals usage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Modules</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>SPI3</t>
+  </si>
+  <si>
+    <t>Slave</t>
+  </si>
+  <si>
+    <t>USART2</t>
+  </si>
+  <si>
+    <t>PA2-3</t>
   </si>
 </sst>
 </file>
@@ -112,7 +121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +173,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -180,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -192,37 +207,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:R18"/>
+  <dimension ref="B3:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,328 +563,358 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7" t="s">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7" t="s">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="10" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2</v>
-      </c>
-      <c r="F13" s="2">
-        <v>3</v>
-      </c>
-      <c r="G13" s="2">
-        <v>4</v>
-      </c>
-      <c r="H13" s="2">
-        <v>5</v>
-      </c>
-      <c r="I13" s="2">
-        <v>6</v>
-      </c>
-      <c r="J13" s="2">
-        <v>7</v>
-      </c>
-      <c r="K13" s="2">
-        <v>8</v>
-      </c>
-      <c r="L13" s="2">
-        <v>9</v>
-      </c>
-      <c r="M13" s="2">
-        <v>10</v>
-      </c>
-      <c r="N13" s="2">
-        <v>11</v>
-      </c>
-      <c r="O13" s="2">
-        <v>12</v>
-      </c>
-      <c r="P13" s="2">
-        <v>13</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>14</v>
-      </c>
-      <c r="R13" s="2">
-        <v>15</v>
-      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>4</v>
+      </c>
+      <c r="H14" s="2">
+        <v>5</v>
+      </c>
+      <c r="I14" s="2">
+        <v>6</v>
+      </c>
+      <c r="J14" s="2">
+        <v>7</v>
+      </c>
+      <c r="K14" s="2">
+        <v>8</v>
+      </c>
+      <c r="L14" s="2">
+        <v>9</v>
+      </c>
+      <c r="M14" s="2">
+        <v>10</v>
+      </c>
+      <c r="N14" s="2">
+        <v>11</v>
+      </c>
+      <c r="O14" s="2">
+        <v>12</v>
+      </c>
+      <c r="P14" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>14</v>
+      </c>
+      <c r="R14" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
+        <v>19</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
+        <v>20</v>
+      </c>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C19" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="26">
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:K9"/>
-    <mergeCell ref="L9:R9"/>
-    <mergeCell ref="B12:R12"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D6:K6"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="D8:K8"/>
     <mergeCell ref="L3:R3"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="L5:R5"/>
     <mergeCell ref="L6:R6"/>
     <mergeCell ref="L7:R7"/>
+    <mergeCell ref="D10:K10"/>
+    <mergeCell ref="L10:R10"/>
+    <mergeCell ref="B13:R13"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="D8:K8"/>
     <mergeCell ref="L8:R8"/>
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D4:K4"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="L9:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>